<commit_message>
import export tanah, gedung, kendaraan fix
</commit_message>
<xml_diff>
--- a/public/templates/template_aset_gedung.xlsx
+++ b/public/templates/template_aset_gedung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\bismillah_sip_aset\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52A4300-9157-4766-BF6B-A713B80A7B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF868AE2-675F-4896-95D0-91328BB91EE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{704EB8C1-9152-478B-B06B-65132D1E22AA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{704EB8C1-9152-478B-B06B-65132D1E22AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>id_status_aset</t>
   </si>
@@ -144,10 +144,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33764376-374A-447A-BA2C-A835B6C3BE19}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,7 +487,7 @@
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -534,9 +533,8 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -576,8 +574,8 @@
       <c r="M2" t="s">
         <v>24</v>
       </c>
-      <c r="N2" t="s">
-        <v>23</v>
+      <c r="N2">
+        <v>0</v>
       </c>
       <c r="O2" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
show detail aset fix
</commit_message>
<xml_diff>
--- a/public/templates/template_aset_gedung.xlsx
+++ b/public/templates/template_aset_gedung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\bismillah_sip_aset\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF868AE2-675F-4896-95D0-91328BB91EE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F112E0-F5DD-42F5-883D-45C72D189E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{704EB8C1-9152-478B-B06B-65132D1E22AA}"/>
   </bookViews>
@@ -75,12 +75,6 @@
     <t>Tersedia</t>
   </si>
   <si>
-    <t>02.02.0001</t>
-  </si>
-  <si>
-    <t>Kantor PUSDIKLAT Kendalisada</t>
-  </si>
-  <si>
     <t>23/11/2023</t>
   </si>
   <si>
@@ -93,9 +87,6 @@
     <t>Beton</t>
   </si>
   <si>
-    <t>Desa Kaliori Kalibagor</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -103,6 +94,15 @@
   </si>
   <si>
     <t>Bantuan Dinas P&amp;K, PEMDA BMS, Kwarnas</t>
+  </si>
+  <si>
+    <t>02.02.0004</t>
+  </si>
+  <si>
+    <t>Kantor Prabubima Tech</t>
+  </si>
+  <si>
+    <t>Pabuaran</t>
   </si>
 </sst>
 </file>
@@ -463,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33764376-374A-447A-BA2C-A835B6C3BE19}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,46 +539,46 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>21</v>
       </c>
       <c r="H2">
         <v>106</v>
       </c>
       <c r="I2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="J2">
         <v>1963</v>
       </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L2">
         <v>175</v>
       </c>
       <c r="M2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N2">
         <v>0</v>
       </c>
       <c r="O2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>